<commit_message>
design uppd 11e feb
</commit_message>
<xml_diff>
--- a/Design/designdokument gammalt och uppdaterat/uppd designdoc (uppd 11e feb).xlsx
+++ b/Design/designdokument gammalt och uppdaterat/uppd designdoc (uppd 11e feb).xlsx
@@ -1315,7 +1315,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
@@ -1422,6 +1422,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1731,8 +1732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A249" workbookViewId="0">
-      <selection activeCell="K265" sqref="K265"/>
+    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
+      <selection activeCell="N270" sqref="N270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7902,7 +7903,7 @@
       <c r="H267" s="61"/>
       <c r="I267" s="61"/>
       <c r="J267" s="63"/>
-      <c r="K267" s="62"/>
+      <c r="K267" s="88"/>
       <c r="L267" s="61"/>
       <c r="M267" s="61"/>
       <c r="N267" s="61"/>

</xml_diff>